<commit_message>
Updated with Extent Listener
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Problem solving with Rohit\Selenium.Data.Driven.CRMWebsite\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D47A7956-CBC2-4899-9C5A-A1489855C4A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C09A058-AA09-4B4D-8696-D3984A1EAFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InsightlyLogInTest" sheetId="1" r:id="rId1"/>
     <sheet name="TaskTest" sheetId="3" r:id="rId2"/>
     <sheet name="NewTaskTest" sheetId="2" r:id="rId3"/>
     <sheet name="LeadTest" sheetId="6" r:id="rId4"/>
-    <sheet name="ContactsTest" sheetId="4" r:id="rId5"/>
-    <sheet name="OrganizationTest" sheetId="5" r:id="rId6"/>
+    <sheet name="OpportunityTest" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
+    <sheet name="ContactsTest" sheetId="4" r:id="rId7"/>
+    <sheet name="OrganizationTest" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
   <si>
     <t>username</t>
   </si>
@@ -182,12 +184,6 @@
     <t>assistant phone</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>Albania</t>
   </si>
   <si>
@@ -288,13 +284,64 @@
   </si>
   <si>
     <t>I am the lead of this team</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>probability</t>
+  </si>
+  <si>
+    <t>bid</t>
+  </si>
+  <si>
+    <t>bidtype</t>
+  </si>
+  <si>
+    <t>pipeline</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>fifty</t>
+  </si>
+  <si>
+    <t>op value</t>
+  </si>
+  <si>
+    <t>USD $</t>
+  </si>
+  <si>
+    <t>Per Day</t>
+  </si>
+  <si>
+    <t>We must bid to win this one</t>
+  </si>
+  <si>
+    <t>Nothing Selected</t>
+  </si>
+  <si>
+    <t>Pulak</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t>leopulak@gmail.com</t>
+  </si>
+  <si>
+    <t>Opportunity Pipeline</t>
+  </si>
+  <si>
+    <t>akd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,6 +351,13 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -332,12 +386,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -707,7 +762,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -742,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472AB716-67BA-4256-8F81-595080B0230F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="J1" workbookViewId="0">
       <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
@@ -777,10 +832,10 @@
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -789,25 +844,25 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="L1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N1" t="s">
         <v>77</v>
       </c>
-      <c r="M1" t="s">
-        <v>78</v>
-      </c>
-      <c r="N1" t="s">
-        <v>79</v>
-      </c>
       <c r="O1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="P1" t="s">
         <v>28</v>
@@ -830,19 +885,19 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D2" t="s">
-        <v>71</v>
-      </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -857,16 +912,16 @@
         <v>324569064</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" t="s">
         <v>80</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>81</v>
-      </c>
-      <c r="M2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N2" t="s">
-        <v>83</v>
       </c>
       <c r="O2" t="s">
         <v>44</v>
@@ -881,10 +936,10 @@
         <v>22304</v>
       </c>
       <c r="S2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="T2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -897,11 +952,113 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11E3B979-D651-4CED-BF87-04F2BD79EC13}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="16.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="26.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.08984375" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037E53F7-234F-461F-8DA0-29D02AC72257}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E614BF-563B-46E6-BAC2-1966A644B9D1}">
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1020,16 +1177,16 @@
         <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>97</v>
       </c>
       <c r="D2" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>98</v>
       </c>
       <c r="F2">
         <v>123456</v>
@@ -1074,7 +1231,7 @@
         <v>12345</v>
       </c>
       <c r="T2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U2" t="s">
         <v>44</v>
@@ -1089,13 +1246,13 @@
         <v>4567</v>
       </c>
       <c r="Y2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Z2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="AA2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1108,12 +1265,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA51909-3FFB-4A8A-BDB5-2AF7E9249367}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1135,16 +1292,16 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
         <v>24</v>
@@ -1156,7 +1313,7 @@
         <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>
@@ -1171,24 +1328,24 @@
         <v>31</v>
       </c>
       <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" t="s">
         <v>60</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" t="s">
         <v>61</v>
-      </c>
-      <c r="O1" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2">
         <v>123456</v>
@@ -1197,7 +1354,7 @@
         <v>5432</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>41</v>
@@ -1206,7 +1363,7 @@
         <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>44</v>
@@ -1221,10 +1378,10 @@
         <v>12345</v>
       </c>
       <c r="L2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
         <v>45</v>
@@ -1236,7 +1393,7 @@
         <v>12345</v>
       </c>
       <c r="Q2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the hashtable and Another Crm website
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Problem solving with Rohit\Selenium.Data.Driven.CRMWebsite\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C09A058-AA09-4B4D-8696-D3984A1EAFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9DD8CE-2662-44C3-9746-0AFBCDEC50E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InsightlyLogInTest" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="NewTaskTest" sheetId="2" r:id="rId3"/>
     <sheet name="LeadTest" sheetId="6" r:id="rId4"/>
     <sheet name="OpportunityTest" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
+    <sheet name="cogmentoLoginTest" sheetId="8" r:id="rId6"/>
     <sheet name="ContactsTest" sheetId="4" r:id="rId7"/>
     <sheet name="OrganizationTest" sheetId="5" r:id="rId8"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
   <si>
     <t>username</t>
   </si>
@@ -94,12 +94,6 @@
     <t>homephone</t>
   </si>
   <si>
-    <t xml:space="preserve">mobile phone </t>
-  </si>
-  <si>
-    <t>other phone</t>
-  </si>
-  <si>
     <t>Assistant name</t>
   </si>
   <si>
@@ -136,21 +130,9 @@
     <t>other city</t>
   </si>
   <si>
-    <t>othr state</t>
-  </si>
-  <si>
-    <t>oth pos code</t>
-  </si>
-  <si>
-    <t>other cou</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
-    <t>tag list</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -181,9 +163,6 @@
     <t>Mr.</t>
   </si>
   <si>
-    <t>assistant phone</t>
-  </si>
-  <si>
     <t>Albania</t>
   </si>
   <si>
@@ -196,9 +175,6 @@
     <t>Self</t>
   </si>
   <si>
-    <t>Phone</t>
-  </si>
-  <si>
     <t>website</t>
   </si>
   <si>
@@ -208,30 +184,12 @@
     <t>www.website.com</t>
   </si>
   <si>
-    <t>billing st</t>
-  </si>
-  <si>
-    <t>shipping city</t>
-  </si>
-  <si>
-    <t>shipping state</t>
-  </si>
-  <si>
-    <t>shipping country</t>
-  </si>
-  <si>
-    <t>shipping post code</t>
-  </si>
-  <si>
     <t>progress</t>
   </si>
   <si>
     <t>no description</t>
   </si>
   <si>
-    <t>no tag</t>
-  </si>
-  <si>
     <t xml:space="preserve">morning view lane </t>
   </si>
   <si>
@@ -334,7 +292,58 @@
     <t>Opportunity Pipeline</t>
   </si>
   <si>
-    <t>akd</t>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>billing</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>postcode</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>scity</t>
+  </si>
+  <si>
+    <t>sstate</t>
+  </si>
+  <si>
+    <t>spcode</t>
+  </si>
+  <si>
+    <t>scountry</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mobilephone </t>
+  </si>
+  <si>
+    <t>otherphone</t>
+  </si>
+  <si>
+    <t>assistantphone</t>
+  </si>
+  <si>
+    <t>other state</t>
+  </si>
+  <si>
+    <t>other country</t>
+  </si>
+  <si>
+    <t>other post code</t>
   </si>
 </sst>
 </file>
@@ -677,7 +686,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -762,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
@@ -798,11 +807,12 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="2" max="2" width="11.7265625" customWidth="1"/>
     <col min="5" max="5" width="14.90625" customWidth="1"/>
     <col min="7" max="7" width="13.1796875" customWidth="1"/>
     <col min="8" max="8" width="15.6328125" customWidth="1"/>
@@ -820,22 +830,22 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
         <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
         <v>17</v>
@@ -844,60 +854,60 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K1" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="L1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>29</v>
       </c>
-      <c r="R1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S1" t="s">
-        <v>31</v>
-      </c>
       <c r="T1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>2</v>
@@ -912,34 +922,34 @@
         <v>324569064</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="N2" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="O2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="P2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="Q2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="R2">
         <v>22304</v>
       </c>
       <c r="S2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="T2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -972,54 +982,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C1" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="H1" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>10000</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1030,35 +1040,48 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037E53F7-234F-461F-8DA0-29D02AC72257}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="12.90625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{EC1C7B18-6566-410A-947A-BE6E7DD83A64}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E614BF-563B-46E6-BAC2-1966A644B9D1}">
-  <dimension ref="A1:AA2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1089,9 +1112,9 @@
     <col min="26" max="26" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
@@ -1112,81 +1135,78 @@
         <v>19</v>
       </c>
       <c r="H1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>23</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>25</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>26</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>28</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>29</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>30</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>31</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X1" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z1" t="s">
         <v>32</v>
       </c>
-      <c r="V1" t="s">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="W1" t="s">
-        <v>34</v>
-      </c>
-      <c r="X1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="F2">
         <v>123456</v>
@@ -1204,55 +1224,52 @@
         <v>543322</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L2">
         <v>7890</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="O2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="P2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="Q2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="R2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="S2">
         <v>12345</v>
       </c>
       <c r="T2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="U2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="W2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="X2">
         <v>4567</v>
       </c>
       <c r="Y2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z2" t="s">
         <v>51</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1269,12 +1286,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA51909-3FFB-4A8A-BDB5-2AF7E9249367}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.36328125" customWidth="1"/>
     <col min="5" max="5" width="20.54296875" customWidth="1"/>
     <col min="6" max="6" width="22.54296875" customWidth="1"/>
@@ -1284,68 +1302,69 @@
     <col min="10" max="10" width="18.453125" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
     <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" customWidth="1"/>
     <col min="14" max="14" width="16.54296875" customWidth="1"/>
     <col min="15" max="15" width="19.6328125" customWidth="1"/>
-    <col min="16" max="16" width="24.26953125" customWidth="1"/>
+    <col min="16" max="16" width="8.81640625" customWidth="1"/>
     <col min="17" max="17" width="14.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="I1" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="J1" t="s">
-        <v>29</v>
+        <v>96</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="L1" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="M1" t="s">
-        <v>58</v>
+        <v>97</v>
       </c>
       <c r="N1" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="O1" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="P1" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="Q1" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>123456</v>
@@ -1354,46 +1373,46 @@
         <v>5432</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K2">
         <v>12345</v>
       </c>
       <c r="L2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="N2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="P2">
         <v>12345</v>
       </c>
       <c r="Q2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifed Extent report and some other files
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Problem solving with Rohit\Selenium.Data.Driven.CRMWebsite\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9DD8CE-2662-44C3-9746-0AFBCDEC50E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB6233E9-83D3-4ADA-B1DC-6C6309D5FCAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InsightlyLogInTest" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="LeadTest" sheetId="6" r:id="rId4"/>
     <sheet name="OpportunityTest" sheetId="7" r:id="rId5"/>
     <sheet name="cogmentoLoginTest" sheetId="8" r:id="rId6"/>
-    <sheet name="ContactsTest" sheetId="4" r:id="rId7"/>
-    <sheet name="OrganizationTest" sheetId="5" r:id="rId8"/>
+    <sheet name="calenderTest" sheetId="9" r:id="rId7"/>
+    <sheet name="ContactsTest" sheetId="4" r:id="rId8"/>
+    <sheet name="contactTest" sheetId="12" r:id="rId9"/>
+    <sheet name="OrganizationTest" sheetId="5" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="138">
   <si>
     <t>username</t>
   </si>
@@ -344,6 +346,108 @@
   </si>
   <si>
     <t>other post code</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>deal</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>alertBefore</t>
+  </si>
+  <si>
+    <t>alertvia</t>
+  </si>
+  <si>
+    <t>reminder</t>
+  </si>
+  <si>
+    <t>participants</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>20/06/2020 20:00</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>This is the first Event</t>
+  </si>
+  <si>
+    <t>Alexandria</t>
+  </si>
+  <si>
+    <t>100 percent</t>
+  </si>
+  <si>
+    <t>Difficult</t>
+  </si>
+  <si>
+    <t>Not yet</t>
+  </si>
+  <si>
+    <t>1 Hour</t>
+  </si>
+  <si>
+    <t>SMS</t>
+  </si>
+  <si>
+    <t>Alak &amp; Toma</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>Hashtag</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>Kanti</t>
+  </si>
+  <si>
+    <t>Iskcon</t>
+  </si>
+  <si>
+    <t>pulak.dental@gmail.com</t>
+  </si>
+  <si>
+    <t>business email</t>
+  </si>
+  <si>
+    <t>pulak.dental@dentalpoint.com</t>
+  </si>
+  <si>
+    <t>Hello How are you</t>
+  </si>
+  <si>
+    <t>5335 Duke St</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>zipcode</t>
   </si>
 </sst>
 </file>
@@ -719,6 +823,150 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA51909-3FFB-4A8A-BDB5-2AF7E9249367}">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="22.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17.54296875" customWidth="1"/>
+    <col min="9" max="9" width="17.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" customWidth="1"/>
+    <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" customWidth="1"/>
+    <col min="14" max="14" width="16.54296875" customWidth="1"/>
+    <col min="15" max="15" width="19.6328125" customWidth="1"/>
+    <col min="16" max="16" width="8.81640625" customWidth="1"/>
+    <col min="17" max="17" width="14.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K1" t="s">
+        <v>90</v>
+      </c>
+      <c r="L1" t="s">
+        <v>91</v>
+      </c>
+      <c r="M1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N1" t="s">
+        <v>92</v>
+      </c>
+      <c r="O1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2">
+        <v>123456</v>
+      </c>
+      <c r="C2">
+        <v>5432</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2">
+        <v>12345</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>12345</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{9E5E7EA4-B034-479B-A51A-6F350C426422}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{94054E4A-93C7-4C74-8F81-4AFB53110C77}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{41E441B5-5407-4F6E-8090-E33616436A3C}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{881DD7DF-7212-4D83-A9DD-3DAD1E365BA4}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37477F2-C6D0-49AB-A8FE-77787C651FEB}">
   <dimension ref="A1:A2"/>
@@ -1042,7 +1290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{037E53F7-234F-461F-8DA0-29D02AC72257}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1077,16 +1325,129 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0BBAE5F-C35E-405D-9E24-61A4ABCA3BFC}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" customWidth="1"/>
+    <col min="2" max="2" width="16.36328125" customWidth="1"/>
+    <col min="3" max="3" width="16.6328125" customWidth="1"/>
+    <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
+    <col min="10" max="10" width="14.90625" customWidth="1"/>
+    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="12" max="12" width="16.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.08984375" customWidth="1"/>
+    <col min="14" max="14" width="11.36328125" customWidth="1"/>
+    <col min="15" max="15" width="12.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" t="s">
+        <v>109</v>
+      </c>
+      <c r="H1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+      <c r="L1" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E614BF-563B-46E6-BAC2-1966A644B9D1}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
+    <col min="2" max="3" width="8.7265625" customWidth="1"/>
     <col min="4" max="4" width="5.7265625" customWidth="1"/>
     <col min="5" max="5" width="16.54296875" customWidth="1"/>
     <col min="6" max="6" width="14.08984375" customWidth="1"/>
@@ -1274,65 +1635,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1116725F-B0EB-4608-8D8B-26FB25449B8A}"/>
+    <hyperlink ref="N2" r:id="rId1" xr:uid="{0D082B77-FA02-4FB5-B626-3E4C1F834DDA}"/>
     <hyperlink ref="M2" r:id="rId2" xr:uid="{8305EBCC-4DC5-4B82-9C72-EA8FB8CF95DA}"/>
-    <hyperlink ref="N2" r:id="rId3" xr:uid="{0D082B77-FA02-4FB5-B626-3E4C1F834DDA}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{1116725F-B0EB-4608-8D8B-26FB25449B8A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DA51909-3FFB-4A8A-BDB5-2AF7E9249367}">
-  <dimension ref="A1:Q2"/>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5B2352-ABB8-49CC-B030-B677F1135C1A}">
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" customWidth="1"/>
-    <col min="5" max="5" width="20.54296875" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="8" max="8" width="17.54296875" customWidth="1"/>
-    <col min="9" max="9" width="17.81640625" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" customWidth="1"/>
-    <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="12" max="12" width="17" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" customWidth="1"/>
-    <col min="14" max="14" width="16.54296875" customWidth="1"/>
-    <col min="15" max="15" width="19.6328125" customWidth="1"/>
-    <col min="16" max="16" width="8.81640625" customWidth="1"/>
-    <col min="17" max="17" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="22.36328125" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" customWidth="1"/>
+    <col min="7" max="7" width="17.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="E1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="I1" t="s">
         <v>89</v>
@@ -1341,86 +1693,48 @@
         <v>96</v>
       </c>
       <c r="K1" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" t="s">
-        <v>92</v>
-      </c>
-      <c r="O1" t="s">
-        <v>93</v>
-      </c>
-      <c r="P1" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2">
-        <v>123456</v>
-      </c>
-      <c r="C2">
-        <v>5432</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
+        <v>82</v>
+      </c>
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" t="s">
+        <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" t="s">
-        <v>38</v>
+        <v>133</v>
+      </c>
+      <c r="G2" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="I2" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>136</v>
       </c>
       <c r="K2">
-        <v>12345</v>
-      </c>
-      <c r="L2" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" t="s">
-        <v>39</v>
-      </c>
-      <c r="O2" t="s">
-        <v>40</v>
-      </c>
-      <c r="P2">
-        <v>12345</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
+        <v>22304</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{9E5E7EA4-B034-479B-A51A-6F350C426422}"/>
-    <hyperlink ref="F2" r:id="rId2" xr:uid="{94054E4A-93C7-4C74-8F81-4AFB53110C77}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{41E441B5-5407-4F6E-8090-E33616436A3C}"/>
-    <hyperlink ref="D2" r:id="rId4" xr:uid="{881DD7DF-7212-4D83-A9DD-3DAD1E365BA4}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{96D38446-FDF4-4B21-B64C-2AC596D7E2DC}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{D6AC2E85-552A-4036-852F-9EEEC0AEE311}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>